<commit_message>
Careers Test Scenario-Fourth Commit
</commit_message>
<xml_diff>
--- a/Careers/target/test-classes/Exceldata/Data.xlsx
+++ b/Careers/target/test-classes/Exceldata/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sprint Implementation\Careers\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F454855-A725-46A2-8D72-ED1246BA0139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA53BFC-A718-4EE8-8EA0-04C4017B1B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{5A44C794-E288-43F0-B7BE-4441423D2C2E}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>